<commit_message>
Sort timeline, edit export pdf and welcome page
</commit_message>
<xml_diff>
--- a/external_files/example_data.xlsx
+++ b/external_files/example_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekty\timeline-app\external_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A3A588-8474-406B-A389-67CB1646554C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4617F584-5215-4DA7-81B3-4CCEDC9D83C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>https://bryan-johnson.medium.com/</t>
   </si>
@@ -245,9 +245,6 @@
     <t>2021-03-09</t>
   </si>
   <si>
-    <t>Evening Byran was fired! Evening Bryan (5pm-10pm) faced a formidable challenge in his daily shift: deciding when, what and how much to eat. For ten years, Evening Bryan overate and gained more than fifty pounds, fueling relentless shame, guilt and malaise. Every night, he failed the marshmallow test; temporarily discounting the future in favor of the here, the now, the carbs, and the sugar... This is Bryans favourite routine now: Eat breakfast at 7 am -&gt; Dinner at 11 am -&gt; Fasting 20 hours a day -&gt; No caffeine or other stimulants -&gt; Discontinue fluids after 4 pm to avoid getting up at night -&gt; 60 minutes of meditation and HRV training</t>
-  </si>
-  <si>
     <t>Upon waking, pre-workout concoction, workout, skincare protocol, breakfast… If you are curious what this looks like in daily practice, look for more.</t>
   </si>
   <si>
@@ -260,10 +257,16 @@
     <t>`With routine measurement of our brains and minds, what questions could we ask and what aspirations can we have?`</t>
   </si>
   <si>
-    <t>Power laws are manifest everywhere, for examle: 80% of internet traffic goes to 20% of websites. They are disproportionately useful if you can harness their energy. When applied to personal behavior, it is likely that 80% of our individual bad behavior is attributable to version of ourselves that exist only in 20% of the time: THE RASCAL 20% VERSION OF YOU CAUSING 80% OF THE DESTRUCTION. To combat this, you can use 5 steps a technique which is used with success.</t>
-  </si>
-  <si>
     <t>Kernel is revolutionizing precision neuroscience. We are using our proprietary, first-in-class neurotechnology to build the world`s most comprehensive portfolio of brain-based biomarkers. Our mission is to accelerate treatment discovery, improve patient outcomes, and transform neuromedicine.</t>
+  </si>
+  <si>
+    <t>Evening Byran was fired! Every night, he failed the marshmallow test; temporarily discounting the future in favor of the here, the now, the carbs, and the sugar... This is Bryans favourite routine now: 2 meals during the day, fasting 20 hours a day, no caffeine or other stimulants etc.</t>
+  </si>
+  <si>
+    <t>Power laws are manifest everywhere. They are disproportionately useful if you can harness their energy. When applied to personal behavior, it is likely that 80% of our individual bad behavior is attributable to version of ourselves that exist only in 20% of the time.</t>
+  </si>
+  <si>
+    <t>My primary objective with Blueprint is to explore the future of being human. Food, supplements, sleep and exercise are necessary for life, however not the primary motivators for most.</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +347,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -366,18 +375,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -663,28 +672,29 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6:I10"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.453125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="26.453125" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="62.81640625" style="7" customWidth="1"/>
     <col min="6" max="6" width="6.26953125" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -703,15 +713,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -725,18 +735,18 @@
       </c>
       <c r="I2" t="str">
         <f>"INSERT INTO `events` ("&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$F$1&amp;", "&amp;$G$1&amp;") VALUES ('"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"', "&amp;F2&amp;", '"&amp;G2&amp;"');"</f>
-        <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Fired Myself', '2020-08-06', 'Evening Byran was fired! Evening Bryan (5pm-10pm) faced a formidable challenge in his daily shift: deciding when, what and how much to eat. For ten years, Evening Bryan overate and gained more than fifty pounds, fueling relentless shame, guilt and malaise. Every night, he failed the marshmallow test; temporarily discounting the future in favor of the here, the now, the carbs, and the sugar... This is Bryans favourite routine now: Eat breakfast at 7 am -&gt; Dinner at 11 am -&gt; Fasting 20 hours a day -&gt; No caffeine or other stimulants -&gt; Discontinue fluids after 4 pm to avoid getting up at night -&gt; 60 minutes of meditation and HRV training', 6, 'https://medium.com/future-literacy/i-fired-myself-d74e2228e873');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+        <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Fired Myself', '2020-08-06', 'Evening Byran was fired! Every night, he failed the marshmallow test; temporarily discounting the future in favor of the here, the now, the carbs, and the sugar... This is Bryans favourite routine now: 2 meals during the day, fasting 20 hours a day, no caffeine or other stimulants etc.', 6, 'https://medium.com/future-literacy/i-fired-myself-d74e2228e873');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>46</v>
+      <c r="D3" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -753,14 +763,14 @@
         <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Kernel on Psychedelics', '2021-01-26', 'Kernel is revolutionizing precision neuroscience. We are using our proprietary, first-in-class neurotechnology to build the world`s most comprehensive portfolio of brain-based biomarkers. Our mission is to accelerate treatment discovery, improve patient outcomes, and transform neuromedicine.', 6, 'https://medium.com/future-literacy/kernel-on-psychedelics-84af60eaf133');</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="4" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
@@ -778,15 +788,15 @@
         <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Project Blueprint', '2023-10-13', 'Aim of project is to measure all 70 organs of Bryan body and then maximally reverse the quantified biological age of each. This started when Bryan fired himself last year from being authorized to make decision about what and how much to eat.', 6, 'https://medium.com/future-literacy/kernel-on-psychedelics-84af60eaf133');</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="5" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
-        <v>41</v>
+      <c r="D5" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -803,12 +813,15 @@
         <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Blueprint Morning Routine', '2023-01-12', 'Upon waking, pre-workout concoction, workout, skincare protocol, breakfast… If you are curious what this looks like in daily practice, look for more.', 6, 'https://medium.com/future-literacy/blueprint-morning-routine-ffdce2654b76');</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="6" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -822,18 +835,18 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Result From Nine Months on Blueprint', '2022-03-08', '', 6, 'https://medium.com/future-literacy/results-from-nine-months-on-blueprint-3e1d6798e57b');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+        <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Result From Nine Months on Blueprint', '2022-03-08', 'My primary objective with Blueprint is to explore the future of being human. Food, supplements, sleep and exercise are necessary for life, however not the primary motivators for most.', 6, 'https://medium.com/future-literacy/results-from-nine-months-on-blueprint-3e1d6798e57b');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>45</v>
+      <c r="D7" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -847,18 +860,18 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('The Power Law of Good Behavior', '2023-11-17', 'Power laws are manifest everywhere, for examle: 80% of internet traffic goes to 20% of websites. They are disproportionately useful if you can harness their energy. When applied to personal behavior, it is likely that 80% of our individual bad behavior is attributable to version of ourselves that exist only in 20% of the time: THE RASCAL 20% VERSION OF YOU CAUSING 80% OF THE DESTRUCTION. To combat this, you can use 5 steps a technique which is used with success.', 6, 'https://medium.com/future-literacy/the-power-law-of-good-behavior-586bd2a05aeb');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+        <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('The Power Law of Good Behavior', '2023-11-17', 'Power laws are manifest everywhere. They are disproportionately useful if you can harness their energy. When applied to personal behavior, it is likely that 80% of our individual bad behavior is attributable to version of ourselves that exist only in 20% of the time.', 6, 'https://medium.com/future-literacy/the-power-law-of-good-behavior-586bd2a05aeb');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>44</v>
+      <c r="D8" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -875,15 +888,15 @@
         <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('New Era of Exploring the Brain', '2023-03-07', '`With routine measurement of our brains and minds, what questions could we ask and what aspirations can we have?`', 6, 'https://bryan-johnson.medium.com/a-new-era-for-exploring-the-brain-1a413d7ecc30');</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>42</v>
+      <c r="D9" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -900,15 +913,15 @@
         <v>INSERT INTO `events` (name, event_date, description, category_id, link) VALUES ('Age 45, I Now Age Slower Than The Average 10 Year Old', '2023-04-07', 'Bryans speed of aging: slower than the average 10 years old, slower than 88% of 18 years olds, in the 94th percentile compared to those chronologically aned 45.', 6, 'https://medium.com/future-literacy/at-45-i-now-age-slower-than-the-average-10-year-old-6932448fc608');</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>43</v>
+      <c r="D10" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>

</xml_diff>